<commit_message>
add and update all testcases and test suites
</commit_message>
<xml_diff>
--- a/Data Files/Raw Data/CO Test.xlsx
+++ b/Data Files/Raw Data/CO Test.xlsx
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t xml:space="preserve">First Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postal Code</t>
+    <t xml:space="preserve">First_Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last_Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postal_Code</t>
   </si>
   <si>
     <t xml:space="preserve">atikah</t>
@@ -169,7 +169,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>